<commit_message>
Part 1 of Question 2
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA14\Projects\lookups-da14-Hannah00Donnelly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABDA806-1334-489C-8194-6695B6537C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5396BC-230F-4892-9573-232DD6468EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24060" yWindow="285" windowWidth="24000" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,12 +1270,16 @@
         <v>341243679.13</v>
       </c>
       <c r="D2" s="10">
-        <f>B2-C2</f>
-        <v>15396420.870000005</v>
+        <f>C2-B2</f>
+        <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
-        <f>IFERROR((B2-C2)/B2,"-")</f>
-        <v>4.3170750765267295E-2</v>
+        <f>IFERROR((D2)/B2,"-")</f>
+        <v>-4.3170750765267295E-2</v>
+      </c>
+      <c r="F2">
+        <f>IFERROR(_xlfn.RANK.EQ(E2,E$2:E$52,0),"N/A")</f>
+        <v>35</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -1284,12 +1288,16 @@
         <v>346340810.81999999</v>
       </c>
       <c r="I2" s="10">
-        <f>G2-H2</f>
-        <v>36344389.180000007</v>
+        <f>H2-G2</f>
+        <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
-        <f>IFERROR((G2-H2)/G2,"-")</f>
-        <v>9.4972027086493035E-2</v>
+        <f>IFERROR((I2)/G2,"-")</f>
+        <v>-9.4972027086493035E-2</v>
+      </c>
+      <c r="K2">
+        <f>IFERROR(_xlfn.RANK.EQ(J2,J$2:J$52,0),"N/A")</f>
+        <v>39</v>
       </c>
       <c r="L2">
         <v>376548600</v>
@@ -1298,12 +1306,16 @@
         <v>355279492.22999901</v>
       </c>
       <c r="N2" s="10">
-        <f>L2-M2</f>
-        <v>21269107.770000994</v>
+        <f>M2-L2</f>
+        <v>-21269107.770000994</v>
       </c>
       <c r="O2" s="5">
-        <f>IFERROR((L2-M2)/L2,"-")</f>
-        <v>5.6484362894991494E-2</v>
+        <f>IFERROR((N2)/L2,"-")</f>
+        <v>-5.6484362894991494E-2</v>
+      </c>
+      <c r="P2">
+        <f>IFERROR(_xlfn.RANK.EQ(O2,O$2:O$52,0),"N/A")</f>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -1317,12 +1329,16 @@
         <v>321214.59000000003</v>
       </c>
       <c r="D3" s="10">
-        <f t="shared" ref="D3:D52" si="0">B3-C3</f>
-        <v>7585.4099999999744</v>
+        <f>C3-B3</f>
+        <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E52" si="1">IFERROR((B3-C3)/B3,"-")</f>
-        <v>2.3069981751824741E-2</v>
+        <f>IFERROR((D3)/B3,"-")</f>
+        <v>-2.3069981751824741E-2</v>
+      </c>
+      <c r="F3">
+        <f>IFERROR(_xlfn.RANK.EQ(E3,E$2:E$52,0),"N/A")</f>
+        <v>27</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -1331,12 +1347,16 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3" s="10">
-        <f t="shared" ref="I3:I52" si="2">G3-H3</f>
-        <v>22366.290000001027</v>
+        <f>H3-G3</f>
+        <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="3">IFERROR((G3-H3)/G3,"-")</f>
-        <v>6.6804928315415249E-2</v>
+        <f>IFERROR((I3)/G3,"-")</f>
+        <v>-6.6804928315415249E-2</v>
+      </c>
+      <c r="K3">
+        <f>IFERROR(_xlfn.RANK.EQ(J3,J$2:J$52,0),"N/A")</f>
+        <v>35</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -1345,12 +1365,16 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3" s="10">
-        <f t="shared" ref="N3:N52" si="4">L3-M3</f>
-        <v>436.96000000002095</v>
+        <f>M3-L3</f>
+        <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="5">IFERROR((L3-M3)/L3,"-")</f>
-        <v>1.3540749922529313E-3</v>
+        <f>IFERROR((N3)/L3,"-")</f>
+        <v>-1.3540749922529313E-3</v>
+      </c>
+      <c r="P3">
+        <f>IFERROR(_xlfn.RANK.EQ(O3,O$2:O$52,0),"N/A")</f>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -1364,12 +1388,16 @@
         <v>3115157.5599999898</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" si="0"/>
-        <v>15442.440000010189</v>
+        <f>C4-B4</f>
+        <v>-15442.440000010189</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="1"/>
-        <v>4.9327413275443007E-3</v>
+        <f>IFERROR((D4)/B4,"-")</f>
+        <v>-4.9327413275443007E-3</v>
+      </c>
+      <c r="F4">
+        <f>IFERROR(_xlfn.RANK.EQ(E4,E$2:E$52,0),"N/A")</f>
+        <v>7</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -1378,12 +1406,16 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4" s="10">
-        <f t="shared" si="2"/>
-        <v>62606.790000009816</v>
+        <f>H4-G4</f>
+        <v>-62606.790000009816</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="3"/>
-        <v>1.7141743558856015E-2</v>
+        <f>IFERROR((I4)/G4,"-")</f>
+        <v>-1.7141743558856015E-2</v>
+      </c>
+      <c r="K4">
+        <f>IFERROR(_xlfn.RANK.EQ(J4,J$2:J$52,0),"N/A")</f>
+        <v>13</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -1392,12 +1424,16 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4" s="10">
-        <f t="shared" si="4"/>
-        <v>97416.950000009965</v>
+        <f>M4-L4</f>
+        <v>-97416.950000009965</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="5"/>
-        <v>2.6599210899959033E-2</v>
+        <f>IFERROR((N4)/L4,"-")</f>
+        <v>-2.6599210899959033E-2</v>
+      </c>
+      <c r="P4">
+        <f>IFERROR(_xlfn.RANK.EQ(O4,O$2:O$52,0),"N/A")</f>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -1411,12 +1447,16 @@
         <v>6947552.6699999999</v>
       </c>
       <c r="D5" s="10">
-        <f t="shared" si="0"/>
-        <v>723147.33000000007</v>
+        <f>C5-B5</f>
+        <v>-723147.33000000007</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="1"/>
-        <v>9.4273968477453174E-2</v>
+        <f>IFERROR((D5)/B5,"-")</f>
+        <v>-9.4273968477453174E-2</v>
+      </c>
+      <c r="F5">
+        <f>IFERROR(_xlfn.RANK.EQ(E5,E$2:E$52,0),"N/A")</f>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -1425,12 +1465,16 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5" s="10">
-        <f t="shared" si="2"/>
-        <v>947690.6799999997</v>
+        <f>H5-G5</f>
+        <v>-947690.6799999997</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="3"/>
-        <v>0.118932605449092</v>
+        <f>IFERROR((I5)/G5,"-")</f>
+        <v>-0.118932605449092</v>
+      </c>
+      <c r="K5">
+        <f>IFERROR(_xlfn.RANK.EQ(J5,J$2:J$52,0),"N/A")</f>
+        <v>44</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -1439,12 +1483,16 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5" s="10">
-        <f t="shared" si="4"/>
-        <v>262277.08999999985</v>
+        <f>M5-L5</f>
+        <v>-262277.08999999985</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="5"/>
-        <v>3.3800336357544182E-2</v>
+        <f>IFERROR((N5)/L5,"-")</f>
+        <v>-3.3800336357544182E-2</v>
+      </c>
+      <c r="P5">
+        <f>IFERROR(_xlfn.RANK.EQ(O5,O$2:O$52,0),"N/A")</f>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -1458,12 +1506,16 @@
         <v>385908.52</v>
       </c>
       <c r="D6" s="10">
-        <f t="shared" si="0"/>
-        <v>23391.479999999981</v>
+        <f>C6-B6</f>
+        <v>-23391.479999999981</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="1"/>
-        <v>5.7149963352064452E-2</v>
+        <f>IFERROR((D6)/B6,"-")</f>
+        <v>-5.7149963352064452E-2</v>
+      </c>
+      <c r="F6">
+        <f>IFERROR(_xlfn.RANK.EQ(E6,E$2:E$52,0),"N/A")</f>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1472,12 +1524,16 @@
         <v>427758.64</v>
       </c>
       <c r="I6" s="10">
-        <f t="shared" si="2"/>
-        <v>741.35999999998603</v>
+        <f>H6-G6</f>
+        <v>-741.35999999998603</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="3"/>
-        <v>1.7301283547257551E-3</v>
+        <f>IFERROR((I6)/G6,"-")</f>
+        <v>-1.7301283547257551E-3</v>
+      </c>
+      <c r="K6">
+        <f>IFERROR(_xlfn.RANK.EQ(J6,J$2:J$52,0),"N/A")</f>
+        <v>5</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -1486,12 +1542,16 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6" s="10">
-        <f t="shared" si="4"/>
-        <v>85.710000001010485</v>
+        <f>M6-L6</f>
+        <v>-85.710000001010485</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="5"/>
-        <v>1.925202156356929E-4</v>
+        <f>IFERROR((N6)/L6,"-")</f>
+        <v>-1.925202156356929E-4</v>
+      </c>
+      <c r="P6">
+        <f>IFERROR(_xlfn.RANK.EQ(O6,O$2:O$52,0),"N/A")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -1505,12 +1565,16 @@
         <v>2946071.21</v>
       </c>
       <c r="D7" s="10">
-        <f t="shared" si="0"/>
-        <v>382928.79000000004</v>
+        <f>C7-B7</f>
+        <v>-382928.79000000004</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.11502817362571344</v>
+        <f>IFERROR((D7)/B7,"-")</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F7">
+        <f>IFERROR(_xlfn.RANK.EQ(E7,E$2:E$52,0),"N/A")</f>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -1519,12 +1583,16 @@
         <v>3051483.41</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" si="2"/>
-        <v>339416.58999999985</v>
+        <f>H7-G7</f>
+        <v>-339416.58999999985</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="3"/>
-        <v>0.10009631366303927</v>
+        <f>IFERROR((I7)/G7,"-")</f>
+        <v>-0.10009631366303927</v>
+      </c>
+      <c r="K7">
+        <f>IFERROR(_xlfn.RANK.EQ(J7,J$2:J$52,0),"N/A")</f>
+        <v>41</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -1533,12 +1601,16 @@
         <v>2946440.08</v>
       </c>
       <c r="N7" s="10">
-        <f t="shared" si="4"/>
-        <v>398759.91999999993</v>
+        <f>M7-L7</f>
+        <v>-398759.91999999993</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="5"/>
-        <v>0.11920361114432618</v>
+        <f>IFERROR((N7)/L7,"-")</f>
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="P7">
+        <f>IFERROR(_xlfn.RANK.EQ(O7,O$2:O$52,0),"N/A")</f>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1552,12 +1624,16 @@
         <v>1315623.30999999</v>
       </c>
       <c r="D8" s="10">
-        <f t="shared" si="0"/>
-        <v>236476.69000000996</v>
+        <f>C8-B8</f>
+        <v>-236476.69000000996</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.15235918433091292</v>
+        <f>IFERROR((D8)/B8,"-")</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="F8">
+        <f>IFERROR(_xlfn.RANK.EQ(E8,E$2:E$52,0),"N/A")</f>
+        <v>48</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -1566,12 +1642,16 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" si="2"/>
-        <v>206794.01000001002</v>
+        <f>H8-G8</f>
+        <v>-206794.01000001002</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="3"/>
-        <v>0.13000189224870184</v>
+        <f>IFERROR((I8)/G8,"-")</f>
+        <v>-0.13000189224870184</v>
+      </c>
+      <c r="K8">
+        <f>IFERROR(_xlfn.RANK.EQ(J8,J$2:J$52,0),"N/A")</f>
+        <v>45</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -1580,12 +1660,16 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8" s="10">
-        <f t="shared" si="4"/>
-        <v>241564.68000000995</v>
+        <f>M8-L8</f>
+        <v>-241564.68000000995</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="5"/>
-        <v>0.15295680364719175</v>
+        <f>IFERROR((N8)/L8,"-")</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="P8">
+        <f>IFERROR(_xlfn.RANK.EQ(O8,O$2:O$52,0),"N/A")</f>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1599,12 +1683,16 @@
         <v>8952825.2799999993</v>
       </c>
       <c r="D9" s="10">
-        <f t="shared" si="0"/>
-        <v>396574.72000000067</v>
+        <f>C9-B9</f>
+        <v>-396574.72000000067</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>4.2417130511048909E-2</v>
+        <f>IFERROR((D9)/B9,"-")</f>
+        <v>-4.2417130511048909E-2</v>
+      </c>
+      <c r="F9">
+        <f>IFERROR(_xlfn.RANK.EQ(E9,E$2:E$52,0),"N/A")</f>
+        <v>33</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1613,12 +1701,16 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9" s="10">
-        <f t="shared" si="2"/>
-        <v>1144640.4800000004</v>
+        <f>H9-G9</f>
+        <v>-1144640.4800000004</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="3"/>
-        <v>0.10336567542917005</v>
+        <f>IFERROR((I9)/G9,"-")</f>
+        <v>-0.10336567542917005</v>
+      </c>
+      <c r="K9">
+        <f>IFERROR(_xlfn.RANK.EQ(J9,J$2:J$52,0),"N/A")</f>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -1627,12 +1719,16 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9" s="10">
-        <f t="shared" si="4"/>
-        <v>796900.47000000998</v>
+        <f>M9-L9</f>
+        <v>-796900.47000000998</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="5"/>
-        <v>7.3852043000788653E-2</v>
+        <f>IFERROR((N9)/L9,"-")</f>
+        <v>-7.3852043000788653E-2</v>
+      </c>
+      <c r="P9">
+        <f>IFERROR(_xlfn.RANK.EQ(O9,O$2:O$52,0),"N/A")</f>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1646,12 +1742,16 @@
         <v>407090.37</v>
       </c>
       <c r="D10" s="10">
-        <f t="shared" si="0"/>
-        <v>36209.630000000005</v>
+        <f>C10-B10</f>
+        <v>-36209.630000000005</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>8.1681998646514792E-2</v>
+        <f>IFERROR((D10)/B10,"-")</f>
+        <v>-8.1681998646514792E-2</v>
+      </c>
+      <c r="F10">
+        <f>IFERROR(_xlfn.RANK.EQ(E10,E$2:E$52,0),"N/A")</f>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1660,12 +1760,16 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10" s="10">
-        <f t="shared" si="2"/>
-        <v>27292.159999999974</v>
+        <f>H10-G10</f>
+        <v>-27292.159999999974</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="3"/>
-        <v>5.5113408723747932E-2</v>
+        <f>IFERROR((I10)/G10,"-")</f>
+        <v>-5.5113408723747932E-2</v>
+      </c>
+      <c r="K10">
+        <f>IFERROR(_xlfn.RANK.EQ(J10,J$2:J$52,0),"N/A")</f>
+        <v>32</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -1674,12 +1778,16 @@
         <v>478318.92</v>
       </c>
       <c r="N10" s="10">
-        <f t="shared" si="4"/>
-        <v>9181.0800000000163</v>
+        <f>M10-L10</f>
+        <v>-9181.0800000000163</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="5"/>
-        <v>1.883298461538465E-2</v>
+        <f>IFERROR((N10)/L10,"-")</f>
+        <v>-1.883298461538465E-2</v>
+      </c>
+      <c r="P10">
+        <f>IFERROR(_xlfn.RANK.EQ(O10,O$2:O$52,0),"N/A")</f>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1693,12 +1801,16 @@
         <v>0</v>
       </c>
       <c r="D11" s="10">
-        <f t="shared" si="0"/>
+        <f>C11-B11</f>
         <v>0</v>
       </c>
       <c r="E11" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR((D11)/B11,"-")</f>
         <v>-</v>
+      </c>
+      <c r="F11" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(E11,E$2:E$52,0),"N/A")</f>
+        <v>N/A</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1707,12 +1819,16 @@
         <v>0</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="2"/>
+        <f>H11-G11</f>
         <v>0</v>
       </c>
       <c r="J11" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f>IFERROR((I11)/G11,"-")</f>
         <v>-</v>
+      </c>
+      <c r="K11" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(J11,J$2:J$52,0),"N/A")</f>
+        <v>N/A</v>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -1721,12 +1837,16 @@
         <v>63771.91</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" si="4"/>
-        <v>311228.08999999997</v>
+        <f>M11-L11</f>
+        <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="5"/>
-        <v>0.82994157333333329</v>
+        <f>IFERROR((N11)/L11,"-")</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="P11">
+        <f>IFERROR(_xlfn.RANK.EQ(O11,O$2:O$52,0),"N/A")</f>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1740,12 +1860,16 @@
         <v>4066595.33</v>
       </c>
       <c r="D12" s="10">
-        <f t="shared" si="0"/>
-        <v>214304.66999999993</v>
+        <f>C12-B12</f>
+        <v>-214304.66999999993</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>5.0060657805601608E-2</v>
+        <f>IFERROR((D12)/B12,"-")</f>
+        <v>-5.0060657805601608E-2</v>
+      </c>
+      <c r="F12">
+        <f>IFERROR(_xlfn.RANK.EQ(E12,E$2:E$52,0),"N/A")</f>
+        <v>36</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1754,12 +1878,16 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12" s="10">
-        <f t="shared" si="2"/>
-        <v>494844.40000000037</v>
+        <f>H12-G12</f>
+        <v>-494844.40000000037</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="3"/>
-        <v>0.10527708280146378</v>
+        <f>IFERROR((I12)/G12,"-")</f>
+        <v>-0.10527708280146378</v>
+      </c>
+      <c r="K12">
+        <f>IFERROR(_xlfn.RANK.EQ(J12,J$2:J$52,0),"N/A")</f>
+        <v>43</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -1768,12 +1896,16 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12" s="10">
-        <f t="shared" si="4"/>
-        <v>306086.86000000034</v>
+        <f>M12-L12</f>
+        <v>-306086.86000000034</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="5"/>
-        <v>6.5433934755654441E-2</v>
+        <f>IFERROR((N12)/L12,"-")</f>
+        <v>-6.5433934755654441E-2</v>
+      </c>
+      <c r="P12">
+        <f>IFERROR(_xlfn.RANK.EQ(O12,O$2:O$52,0),"N/A")</f>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1787,12 +1919,16 @@
         <v>5772288.3300000001</v>
       </c>
       <c r="D13" s="10">
-        <f t="shared" si="0"/>
-        <v>75511.669999999925</v>
+        <f>C13-B13</f>
+        <v>-75511.669999999925</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2912833886247806E-2</v>
+        <f>IFERROR((D13)/B13,"-")</f>
+        <v>-1.2912833886247806E-2</v>
+      </c>
+      <c r="F13">
+        <f>IFERROR(_xlfn.RANK.EQ(E13,E$2:E$52,0),"N/A")</f>
+        <v>16</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1801,12 +1937,16 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="2"/>
-        <v>314622.06000000983</v>
+        <f>H13-G13</f>
+        <v>-314622.06000000983</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="3"/>
-        <v>5.0552253482656594E-2</v>
+        <f>IFERROR((I13)/G13,"-")</f>
+        <v>-5.0552253482656594E-2</v>
+      </c>
+      <c r="K13">
+        <f>IFERROR(_xlfn.RANK.EQ(J13,J$2:J$52,0),"N/A")</f>
+        <v>31</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -1815,12 +1955,16 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" si="4"/>
-        <v>150323.33000000007</v>
+        <f>M13-L13</f>
+        <v>-150323.33000000007</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="5"/>
-        <v>2.4217184605222895E-2</v>
+        <f>IFERROR((N13)/L13,"-")</f>
+        <v>-2.4217184605222895E-2</v>
+      </c>
+      <c r="P13">
+        <f>IFERROR(_xlfn.RANK.EQ(O13,O$2:O$52,0),"N/A")</f>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -1834,12 +1978,16 @@
         <v>505017.37</v>
       </c>
       <c r="D14" s="10">
-        <f t="shared" si="0"/>
-        <v>6982.6300000000047</v>
+        <f>C14-B14</f>
+        <v>-6982.6300000000047</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>1.3637949218750009E-2</v>
+        <f>IFERROR((D14)/B14,"-")</f>
+        <v>-1.3637949218750009E-2</v>
+      </c>
+      <c r="F14">
+        <f>IFERROR(_xlfn.RANK.EQ(E14,E$2:E$52,0),"N/A")</f>
+        <v>19</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -1848,12 +1996,16 @@
         <v>524402.98</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="2"/>
-        <v>6097.0200000000186</v>
+        <f>H14-G14</f>
+        <v>-6097.0200000000186</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="3"/>
-        <v>1.1492968897266765E-2</v>
+        <f>IFERROR((I14)/G14,"-")</f>
+        <v>-1.1492968897266765E-2</v>
+      </c>
+      <c r="K14">
+        <f>IFERROR(_xlfn.RANK.EQ(J14,J$2:J$52,0),"N/A")</f>
+        <v>9</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -1862,12 +2014,16 @@
         <v>504989.88</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" si="4"/>
-        <v>21210.119999999995</v>
+        <f>M14-L14</f>
+        <v>-21210.119999999995</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="5"/>
-        <v>4.0308095781071827E-2</v>
+        <f>IFERROR((N14)/L14,"-")</f>
+        <v>-4.0308095781071827E-2</v>
+      </c>
+      <c r="P14">
+        <f>IFERROR(_xlfn.RANK.EQ(O14,O$2:O$52,0),"N/A")</f>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1881,12 +2037,16 @@
         <v>156545919.90000001</v>
       </c>
       <c r="D15" s="10">
-        <f t="shared" si="0"/>
-        <v>-496819.90000000596</v>
+        <f>C15-B15</f>
+        <v>496819.90000000596</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>-3.1837408866824991E-3</v>
+        <f>IFERROR((D15)/B15,"-")</f>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="F15">
+        <f>IFERROR(_xlfn.RANK.EQ(E15,E$2:E$52,0),"N/A")</f>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -1895,12 +2055,16 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="2"/>
-        <v>8201410.7500010133</v>
+        <f>H15-G15</f>
+        <v>-8201410.7500010133</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="3"/>
-        <v>4.4532273014072019E-2</v>
+        <f>IFERROR((I15)/G15,"-")</f>
+        <v>-4.4532273014072019E-2</v>
+      </c>
+      <c r="K15">
+        <f>IFERROR(_xlfn.RANK.EQ(J15,J$2:J$52,0),"N/A")</f>
+        <v>25</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -1909,12 +2073,16 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15" s="10">
-        <f t="shared" si="4"/>
-        <v>4502589.1500009894</v>
+        <f>M15-L15</f>
+        <v>-4502589.1500009894</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="5"/>
-        <v>2.3829085727446114E-2</v>
+        <f>IFERROR((N15)/L15,"-")</f>
+        <v>-2.3829085727446114E-2</v>
+      </c>
+      <c r="P15">
+        <f>IFERROR(_xlfn.RANK.EQ(O15,O$2:O$52,0),"N/A")</f>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -1928,12 +2096,16 @@
         <v>6522480.4599999897</v>
       </c>
       <c r="D16" s="10">
-        <f t="shared" si="0"/>
-        <v>78219.540000010282</v>
+        <f>C16-B16</f>
+        <v>-78219.540000010282</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="1"/>
-        <v>1.1850188616360429E-2</v>
+        <f>IFERROR((D16)/B16,"-")</f>
+        <v>-1.1850188616360429E-2</v>
+      </c>
+      <c r="F16">
+        <f>IFERROR(_xlfn.RANK.EQ(E16,E$2:E$52,0),"N/A")</f>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -1942,12 +2114,16 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="2"/>
-        <v>2035.9199999999255</v>
+        <f>H16-G16</f>
+        <v>-2035.9199999999255</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="3"/>
-        <v>2.769017341040361E-4</v>
+        <f>IFERROR((I16)/G16,"-")</f>
+        <v>-2.769017341040361E-4</v>
+      </c>
+      <c r="K16">
+        <f>IFERROR(_xlfn.RANK.EQ(J16,J$2:J$52,0),"N/A")</f>
+        <v>3</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -1956,15 +2132,19 @@
         <v>7397093</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="4"/>
-        <v>107</v>
+        <f>M16-L16</f>
+        <v>-107</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="5"/>
-        <v>1.4464932677229222E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N16)/L16,"-")</f>
+        <v>-1.4464932677229222E-5</v>
+      </c>
+      <c r="P16">
+        <f>IFERROR(_xlfn.RANK.EQ(O16,O$2:O$52,0),"N/A")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1975,12 +2155,16 @@
         <v>14439480.050000001</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" si="0"/>
-        <v>421319.94999999925</v>
+        <f>C17-B17</f>
+        <v>-421319.94999999925</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="1"/>
-        <v>2.8351094826658003E-2</v>
+        <f>IFERROR((D17)/B17,"-")</f>
+        <v>-2.8351094826658003E-2</v>
+      </c>
+      <c r="F17">
+        <f>IFERROR(_xlfn.RANK.EQ(E17,E$2:E$52,0),"N/A")</f>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -1989,12 +2173,16 @@
         <v>14645233.51</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="2"/>
-        <v>664466.49000000022</v>
+        <f>H17-G17</f>
+        <v>-664466.49000000022</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3401666263871937E-2</v>
+        <f>IFERROR((I17)/G17,"-")</f>
+        <v>-4.3401666263871937E-2</v>
+      </c>
+      <c r="K17">
+        <f>IFERROR(_xlfn.RANK.EQ(J17,J$2:J$52,0),"N/A")</f>
+        <v>24</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -2003,15 +2191,19 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17" s="10">
-        <f t="shared" si="4"/>
-        <v>965742.96000000089</v>
+        <f>M17-L17</f>
+        <v>-965742.96000000089</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="5"/>
-        <v>6.3071811282801551E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N17)/L17,"-")</f>
+        <v>-6.3071811282801551E-2</v>
+      </c>
+      <c r="P17">
+        <f>IFERROR(_xlfn.RANK.EQ(O17,O$2:O$52,0),"N/A")</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2022,12 +2214,16 @@
         <v>2615303.8999999901</v>
       </c>
       <c r="D18" s="10">
-        <f t="shared" si="0"/>
-        <v>149396.10000000987</v>
+        <f>C18-B18</f>
+        <v>-149396.10000000987</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>5.4037002206391245E-2</v>
+        <f>IFERROR((D18)/B18,"-")</f>
+        <v>-5.4037002206391245E-2</v>
+      </c>
+      <c r="F18">
+        <f>IFERROR(_xlfn.RANK.EQ(E18,E$2:E$52,0),"N/A")</f>
+        <v>37</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2036,12 +2232,16 @@
         <v>2671745.94</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="2"/>
-        <v>189254.06000000006</v>
+        <f>H18-G18</f>
+        <v>-189254.06000000006</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="3"/>
-        <v>6.6149619014330668E-2</v>
+        <f>IFERROR((I18)/G18,"-")</f>
+        <v>-6.6149619014330668E-2</v>
+      </c>
+      <c r="K18">
+        <f>IFERROR(_xlfn.RANK.EQ(J18,J$2:J$52,0),"N/A")</f>
+        <v>34</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -2050,15 +2250,19 @@
         <v>2535637.09</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="4"/>
-        <v>374962.91000000015</v>
+        <f>M18-L18</f>
+        <v>-374962.91000000015</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="5"/>
-        <v>0.12882667147667154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N18)/L18,"-")</f>
+        <v>-0.12882667147667154</v>
+      </c>
+      <c r="P18">
+        <f>IFERROR(_xlfn.RANK.EQ(O18,O$2:O$52,0),"N/A")</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2069,12 +2273,16 @@
         <v>8460963.1999999899</v>
       </c>
       <c r="D19" s="10">
-        <f t="shared" si="0"/>
-        <v>376336.80000001006</v>
+        <f>C19-B19</f>
+        <v>-376336.80000001006</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="1"/>
-        <v>4.258504294298146E-2</v>
+        <f>IFERROR((D19)/B19,"-")</f>
+        <v>-4.258504294298146E-2</v>
+      </c>
+      <c r="F19">
+        <f>IFERROR(_xlfn.RANK.EQ(E19,E$2:E$52,0),"N/A")</f>
+        <v>34</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2083,12 +2291,16 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="2"/>
-        <v>721592.76000000909</v>
+        <f>H19-G19</f>
+        <v>-721592.76000000909</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="3"/>
-        <v>7.4289145810384635E-2</v>
+        <f>IFERROR((I19)/G19,"-")</f>
+        <v>-7.4289145810384635E-2</v>
+      </c>
+      <c r="K19">
+        <f>IFERROR(_xlfn.RANK.EQ(J19,J$2:J$52,0),"N/A")</f>
+        <v>37</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -2097,15 +2309,19 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="4"/>
-        <v>576344.08999999985</v>
+        <f>M19-L19</f>
+        <v>-576344.08999999985</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="5"/>
-        <v>6.1687262121374278E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N19)/L19,"-")</f>
+        <v>-6.1687262121374278E-2</v>
+      </c>
+      <c r="P19">
+        <f>IFERROR(_xlfn.RANK.EQ(O19,O$2:O$52,0),"N/A")</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2116,12 +2332,16 @@
         <v>124384360.159999</v>
       </c>
       <c r="D20" s="10">
-        <f t="shared" si="0"/>
-        <v>1539.8400010019541</v>
+        <f>C20-B20</f>
+        <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2379538203300809E-5</v>
+        <f>IFERROR((D20)/B20,"-")</f>
+        <v>-1.2379538203300809E-5</v>
+      </c>
+      <c r="F20">
+        <f>IFERROR(_xlfn.RANK.EQ(E20,E$2:E$52,0),"N/A")</f>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2130,12 +2350,16 @@
         <v>131839624.37</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="2"/>
-        <v>9775.6299999952316</v>
+        <f>H20-G20</f>
+        <v>-9775.6299999952316</v>
       </c>
       <c r="J20" s="5">
-        <f t="shared" si="3"/>
-        <v>7.4142392760188761E-5</v>
+        <f>IFERROR((I20)/G20,"-")</f>
+        <v>-7.4142392760188761E-5</v>
+      </c>
+      <c r="K20">
+        <f>IFERROR(_xlfn.RANK.EQ(J20,J$2:J$52,0),"N/A")</f>
+        <v>2</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -2144,15 +2368,19 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="4"/>
-        <v>116.46000100672245</v>
+        <f>M20-L20</f>
+        <v>-116.46000100672245</v>
       </c>
       <c r="O20" s="5">
-        <f t="shared" si="5"/>
-        <v>8.9158438821450736E-7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N20)/L20,"-")</f>
+        <v>-8.9158438821450736E-7</v>
+      </c>
+      <c r="P20">
+        <f>IFERROR(_xlfn.RANK.EQ(O20,O$2:O$52,0),"N/A")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2163,12 +2391,16 @@
         <v>22408587.5499999</v>
       </c>
       <c r="D21" s="10">
-        <f t="shared" si="0"/>
-        <v>1923512.4500000998</v>
+        <f>C21-B21</f>
+        <v>-1923512.4500000998</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="1"/>
-        <v>7.9052463618023094E-2</v>
+        <f>IFERROR((D21)/B21,"-")</f>
+        <v>-7.9052463618023094E-2</v>
+      </c>
+      <c r="F21">
+        <f>IFERROR(_xlfn.RANK.EQ(E21,E$2:E$52,0),"N/A")</f>
+        <v>40</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2177,12 +2409,16 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="2"/>
-        <v>1841406.370000001</v>
+        <f>H21-G21</f>
+        <v>-1841406.370000001</v>
       </c>
       <c r="J21" s="5">
-        <f t="shared" si="3"/>
-        <v>7.5167420624229556E-2</v>
+        <f>IFERROR((I21)/G21,"-")</f>
+        <v>-7.5167420624229556E-2</v>
+      </c>
+      <c r="K21">
+        <f>IFERROR(_xlfn.RANK.EQ(J21,J$2:J$52,0),"N/A")</f>
+        <v>38</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -2191,15 +2427,19 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="4"/>
-        <v>888926.91000010073</v>
+        <f>M21-L21</f>
+        <v>-888926.91000010073</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="5"/>
-        <v>3.6546762734864152E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N21)/L21,"-")</f>
+        <v>-3.6546762734864152E-2</v>
+      </c>
+      <c r="P21">
+        <f>IFERROR(_xlfn.RANK.EQ(O21,O$2:O$52,0),"N/A")</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2210,12 +2450,16 @@
         <v>11412339.8799999</v>
       </c>
       <c r="D22" s="10">
-        <f t="shared" si="0"/>
-        <v>153660.12000009976</v>
+        <f>C22-B22</f>
+        <v>-153660.12000009976</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="1"/>
-        <v>1.3285502334437123E-2</v>
+        <f>IFERROR((D22)/B22,"-")</f>
+        <v>-1.3285502334437123E-2</v>
+      </c>
+      <c r="F22">
+        <f>IFERROR(_xlfn.RANK.EQ(E22,E$2:E$52,0),"N/A")</f>
+        <v>17</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2224,12 +2468,16 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="2"/>
-        <v>188722.03000009991</v>
+        <f>H22-G22</f>
+        <v>-188722.03000009991</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="3"/>
-        <v>1.5752170574348738E-2</v>
+        <f>IFERROR((I22)/G22,"-")</f>
+        <v>-1.5752170574348738E-2</v>
+      </c>
+      <c r="K22">
+        <f>IFERROR(_xlfn.RANK.EQ(J22,J$2:J$52,0),"N/A")</f>
+        <v>11</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -2238,15 +2486,19 @@
         <v>11934454.77</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="4"/>
-        <v>745.23000000044703</v>
+        <f>M22-L22</f>
+        <v>-745.23000000044703</v>
       </c>
       <c r="O22" s="5">
-        <f t="shared" si="5"/>
-        <v>6.2439674240938325E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N22)/L22,"-")</f>
+        <v>-6.2439674240938325E-5</v>
+      </c>
+      <c r="P22">
+        <f>IFERROR(_xlfn.RANK.EQ(O22,O$2:O$52,0),"N/A")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2257,12 +2509,16 @@
         <v>20036743.4099999</v>
       </c>
       <c r="D23" s="10">
-        <f t="shared" si="0"/>
-        <v>825956.59000010043</v>
+        <f>C23-B23</f>
+        <v>-825956.59000010043</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="1"/>
-        <v>3.9590110100806722E-2</v>
+        <f>IFERROR((D23)/B23,"-")</f>
+        <v>-3.9590110100806722E-2</v>
+      </c>
+      <c r="F23">
+        <f>IFERROR(_xlfn.RANK.EQ(E23,E$2:E$52,0),"N/A")</f>
+        <v>31</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2271,12 +2527,16 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23" s="10">
-        <f t="shared" si="2"/>
-        <v>961673.78000010177</v>
+        <f>H23-G23</f>
+        <v>-961673.78000010177</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" si="3"/>
-        <v>4.2394738976719144E-2</v>
+        <f>IFERROR((I23)/G23,"-")</f>
+        <v>-4.2394738976719144E-2</v>
+      </c>
+      <c r="K23">
+        <f>IFERROR(_xlfn.RANK.EQ(J23,J$2:J$52,0),"N/A")</f>
+        <v>23</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -2285,15 +2545,19 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23" s="10">
-        <f t="shared" si="4"/>
-        <v>601242.55999999866</v>
+        <f>M23-L23</f>
+        <v>-601242.55999999866</v>
       </c>
       <c r="O23" s="5">
-        <f t="shared" si="5"/>
-        <v>2.5892971236375011E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N23)/L23,"-")</f>
+        <v>-2.5892971236375011E-2</v>
+      </c>
+      <c r="P23">
+        <f>IFERROR(_xlfn.RANK.EQ(O23,O$2:O$52,0),"N/A")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2304,12 +2568,16 @@
         <v>904969.19</v>
       </c>
       <c r="D24" s="10">
-        <f t="shared" si="0"/>
-        <v>12230.810000000056</v>
+        <f>C24-B24</f>
+        <v>-12230.810000000056</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="1"/>
-        <v>1.3334943305713101E-2</v>
+        <f>IFERROR((D24)/B24,"-")</f>
+        <v>-1.3334943305713101E-2</v>
+      </c>
+      <c r="F24">
+        <f>IFERROR(_xlfn.RANK.EQ(E24,E$2:E$52,0),"N/A")</f>
+        <v>18</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2318,12 +2586,16 @@
         <v>1067214.42</v>
       </c>
       <c r="I24" s="10">
-        <f t="shared" si="2"/>
-        <v>45485.580000000075</v>
+        <f>H24-G24</f>
+        <v>-45485.580000000075</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="3"/>
-        <v>4.087856565111897E-2</v>
+        <f>IFERROR((I24)/G24,"-")</f>
+        <v>-4.087856565111897E-2</v>
+      </c>
+      <c r="K24">
+        <f>IFERROR(_xlfn.RANK.EQ(J24,J$2:J$52,0),"N/A")</f>
+        <v>21</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -2332,15 +2604,19 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24" s="10">
-        <f t="shared" si="4"/>
-        <v>72.879999999888241</v>
+        <f>M24-L24</f>
+        <v>-72.879999999888241</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="5"/>
-        <v>6.5504224339284781E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N24)/L24,"-")</f>
+        <v>-6.5504224339284781E-5</v>
+      </c>
+      <c r="P24">
+        <f>IFERROR(_xlfn.RANK.EQ(O24,O$2:O$52,0),"N/A")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2351,12 +2627,16 @@
         <v>479149.53</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" si="0"/>
-        <v>4950.4699999999721</v>
+        <f>C25-B25</f>
+        <v>-4950.4699999999721</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0226130964676661E-2</v>
+        <f>IFERROR((D25)/B25,"-")</f>
+        <v>-1.0226130964676661E-2</v>
+      </c>
+      <c r="F25">
+        <f>IFERROR(_xlfn.RANK.EQ(E25,E$2:E$52,0),"N/A")</f>
+        <v>11</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2365,12 +2645,16 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="2"/>
-        <v>8005.7900000010268</v>
+        <f>H25-G25</f>
+        <v>-8005.7900000010268</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="3"/>
-        <v>1.5846773555029746E-2</v>
+        <f>IFERROR((I25)/G25,"-")</f>
+        <v>-1.5846773555029746E-2</v>
+      </c>
+      <c r="K25">
+        <f>IFERROR(_xlfn.RANK.EQ(J25,J$2:J$52,0),"N/A")</f>
+        <v>12</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -2379,15 +2663,19 @@
         <v>494775.1</v>
       </c>
       <c r="N25" s="10">
-        <f t="shared" si="4"/>
-        <v>1724.9000000000233</v>
+        <f>M25-L25</f>
+        <v>-1724.9000000000233</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="5"/>
-        <v>3.4741188318228064E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N25)/L25,"-")</f>
+        <v>-3.4741188318228064E-3</v>
+      </c>
+      <c r="P25">
+        <f>IFERROR(_xlfn.RANK.EQ(O25,O$2:O$52,0),"N/A")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2398,12 +2686,16 @@
         <v>4801960.08</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" si="0"/>
-        <v>447839.91999999993</v>
+        <f>C26-B26</f>
+        <v>-447839.91999999993</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="1"/>
-        <v>8.5306091660634673E-2</v>
+        <f>IFERROR((D26)/B26,"-")</f>
+        <v>-8.5306091660634673E-2</v>
+      </c>
+      <c r="F26">
+        <f>IFERROR(_xlfn.RANK.EQ(E26,E$2:E$52,0),"N/A")</f>
+        <v>44</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2412,12 +2704,16 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" si="2"/>
-        <v>319870.97000000998</v>
+        <f>H26-G26</f>
+        <v>-319870.97000000998</v>
       </c>
       <c r="J26" s="5">
-        <f t="shared" si="3"/>
-        <v>5.8776040939327839E-2</v>
+        <f>IFERROR((I26)/G26,"-")</f>
+        <v>-5.8776040939327839E-2</v>
+      </c>
+      <c r="K26">
+        <f>IFERROR(_xlfn.RANK.EQ(J26,J$2:J$52,0),"N/A")</f>
+        <v>33</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -2426,15 +2722,19 @@
         <v>5117235.21</v>
       </c>
       <c r="N26" s="10">
-        <f t="shared" si="4"/>
-        <v>313464.79000000004</v>
+        <f>M26-L26</f>
+        <v>-313464.79000000004</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" si="5"/>
-        <v>5.7720881286022069E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N26)/L26,"-")</f>
+        <v>-5.7720881286022069E-2</v>
+      </c>
+      <c r="P26">
+        <f>IFERROR(_xlfn.RANK.EQ(O26,O$2:O$52,0),"N/A")</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2445,12 +2745,16 @@
         <v>0</v>
       </c>
       <c r="D27" s="10">
-        <f t="shared" si="0"/>
+        <f>C27-B27</f>
         <v>0</v>
       </c>
       <c r="E27" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR((D27)/B27,"-")</f>
         <v>-</v>
+      </c>
+      <c r="F27" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(E27,E$2:E$52,0),"N/A")</f>
+        <v>N/A</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2459,12 +2763,16 @@
         <v>0</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="2"/>
+        <f>H27-G27</f>
         <v>0</v>
       </c>
       <c r="J27" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f>IFERROR((I27)/G27,"-")</f>
         <v>-</v>
+      </c>
+      <c r="K27" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(J27,J$2:J$52,0),"N/A")</f>
+        <v>N/A</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -2473,15 +2781,19 @@
         <v>0</v>
       </c>
       <c r="N27" s="10">
-        <f t="shared" si="4"/>
+        <f>M27-L27</f>
         <v>0</v>
       </c>
       <c r="O27" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f>IFERROR((N27)/L27,"-")</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(O27,O$2:O$52,0),"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2492,12 +2804,16 @@
         <v>1250442.02</v>
       </c>
       <c r="D28" s="10">
-        <f t="shared" si="0"/>
-        <v>132457.97999999998</v>
+        <f>C28-B28</f>
+        <v>-132457.97999999998</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="1"/>
-        <v>9.5782760864849215E-2</v>
+        <f>IFERROR((D28)/B28,"-")</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
+      <c r="F28">
+        <f>IFERROR(_xlfn.RANK.EQ(E28,E$2:E$52,0),"N/A")</f>
+        <v>46</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2506,12 +2822,16 @@
         <v>1281335.23</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="2"/>
-        <v>264364.77</v>
+        <f>H28-G28</f>
+        <v>-264364.77</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="3"/>
-        <v>0.17103239309050916</v>
+        <f>IFERROR((I28)/G28,"-")</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="K28">
+        <f>IFERROR(_xlfn.RANK.EQ(J28,J$2:J$52,0),"N/A")</f>
+        <v>47</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -2520,15 +2840,19 @@
         <v>1393285.06</v>
       </c>
       <c r="N28" s="10">
-        <f t="shared" si="4"/>
-        <v>132614.93999999994</v>
+        <f>M28-L28</f>
+        <v>-132614.93999999994</v>
       </c>
       <c r="O28" s="5">
-        <f t="shared" si="5"/>
-        <v>8.6909325643882263E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N28)/L28,"-")</f>
+        <v>-8.6909325643882263E-2</v>
+      </c>
+      <c r="P28">
+        <f>IFERROR(_xlfn.RANK.EQ(O28,O$2:O$52,0),"N/A")</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2539,12 +2863,16 @@
         <v>2523884.71</v>
       </c>
       <c r="D29" s="10">
-        <f t="shared" si="0"/>
-        <v>37915.290000000037</v>
+        <f>C29-B29</f>
+        <v>-37915.290000000037</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="1"/>
-        <v>1.4800253727847622E-2</v>
+        <f>IFERROR((D29)/B29,"-")</f>
+        <v>-1.4800253727847622E-2</v>
+      </c>
+      <c r="F29">
+        <f>IFERROR(_xlfn.RANK.EQ(E29,E$2:E$52,0),"N/A")</f>
+        <v>21</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2553,12 +2881,16 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29" s="10">
-        <f t="shared" si="2"/>
-        <v>114235.56000000983</v>
+        <f>H29-G29</f>
+        <v>-114235.56000000983</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="3"/>
-        <v>4.1099320021590155E-2</v>
+        <f>IFERROR((I29)/G29,"-")</f>
+        <v>-4.1099320021590155E-2</v>
+      </c>
+      <c r="K29">
+        <f>IFERROR(_xlfn.RANK.EQ(J29,J$2:J$52,0),"N/A")</f>
+        <v>22</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -2567,15 +2899,19 @@
         <v>2889864.67</v>
       </c>
       <c r="N29" s="10">
-        <f t="shared" si="4"/>
-        <v>35.330000000074506</v>
+        <f>M29-L29</f>
+        <v>-35.330000000074506</v>
       </c>
       <c r="O29" s="5">
-        <f t="shared" si="5"/>
-        <v>1.2225336516860273E-5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N29)/L29,"-")</f>
+        <v>-1.2225336516860273E-5</v>
+      </c>
+      <c r="P29">
+        <f>IFERROR(_xlfn.RANK.EQ(O29,O$2:O$52,0),"N/A")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2586,12 +2922,16 @@
         <v>12030494.1</v>
       </c>
       <c r="D30" s="10">
-        <f t="shared" si="0"/>
-        <v>101705.90000000037</v>
+        <f>C30-B30</f>
+        <v>-101705.90000000037</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="1"/>
-        <v>8.3831374359143746E-3</v>
+        <f>IFERROR((D30)/B30,"-")</f>
+        <v>-8.3831374359143746E-3</v>
+      </c>
+      <c r="F30">
+        <f>IFERROR(_xlfn.RANK.EQ(E30,E$2:E$52,0),"N/A")</f>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2600,12 +2940,16 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30" s="10">
-        <f t="shared" si="2"/>
-        <v>50385.720000099391</v>
+        <f>H30-G30</f>
+        <v>-50385.720000099391</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="3"/>
-        <v>3.9561962641116366E-3</v>
+        <f>IFERROR((I30)/G30,"-")</f>
+        <v>-3.9561962641116366E-3</v>
+      </c>
+      <c r="K30">
+        <f>IFERROR(_xlfn.RANK.EQ(J30,J$2:J$52,0),"N/A")</f>
+        <v>7</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -2614,15 +2958,19 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30" s="10">
-        <f t="shared" si="4"/>
-        <v>35290.390000000596</v>
+        <f>M30-L30</f>
+        <v>-35290.390000000596</v>
       </c>
       <c r="O30" s="5">
-        <f t="shared" si="5"/>
-        <v>2.7439209100169185E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N30)/L30,"-")</f>
+        <v>-2.7439209100169185E-3</v>
+      </c>
+      <c r="P30">
+        <f>IFERROR(_xlfn.RANK.EQ(O30,O$2:O$52,0),"N/A")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2633,12 +2981,16 @@
         <v>1740827.69</v>
       </c>
       <c r="D31" s="10">
-        <f t="shared" si="0"/>
-        <v>24772.310000000056</v>
+        <f>C31-B31</f>
+        <v>-24772.310000000056</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="1"/>
-        <v>1.4030533529678329E-2</v>
+        <f>IFERROR((D31)/B31,"-")</f>
+        <v>-1.4030533529678329E-2</v>
+      </c>
+      <c r="F31">
+        <f>IFERROR(_xlfn.RANK.EQ(E31,E$2:E$52,0),"N/A")</f>
+        <v>20</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -2647,12 +2999,16 @@
         <v>1762676.85</v>
       </c>
       <c r="I31" s="10">
-        <f t="shared" si="2"/>
-        <v>60623.149999999907</v>
+        <f>H31-G31</f>
+        <v>-60623.149999999907</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="3"/>
-        <v>3.3249136181648611E-2</v>
+        <f>IFERROR((I31)/G31,"-")</f>
+        <v>-3.3249136181648611E-2</v>
+      </c>
+      <c r="K31">
+        <f>IFERROR(_xlfn.RANK.EQ(J31,J$2:J$52,0),"N/A")</f>
+        <v>17</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -2661,15 +3017,19 @@
         <v>1801391.34</v>
       </c>
       <c r="N31" s="10">
-        <f t="shared" si="4"/>
-        <v>69308.659999999916</v>
+        <f>M31-L31</f>
+        <v>-69308.659999999916</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" si="5"/>
-        <v>3.7049585716576634E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N31)/L31,"-")</f>
+        <v>-3.7049585716576634E-2</v>
+      </c>
+      <c r="P31">
+        <f>IFERROR(_xlfn.RANK.EQ(O31,O$2:O$52,0),"N/A")</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2680,12 +3040,16 @@
         <v>5925637.7199999904</v>
       </c>
       <c r="D32" s="10">
-        <f t="shared" si="0"/>
-        <v>73762.280000009574</v>
+        <f>C32-B32</f>
+        <v>-73762.280000009574</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2294942827617691E-2</v>
+        <f>IFERROR((D32)/B32,"-")</f>
+        <v>-1.2294942827617691E-2</v>
+      </c>
+      <c r="F32">
+        <f>IFERROR(_xlfn.RANK.EQ(E32,E$2:E$52,0),"N/A")</f>
+        <v>13</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -2694,12 +3058,16 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32" s="10">
-        <f t="shared" si="2"/>
-        <v>110514.53000000026</v>
+        <f>H32-G32</f>
+        <v>-110514.53000000026</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="3"/>
-        <v>1.7837871035428981E-2</v>
+        <f>IFERROR((I32)/G32,"-")</f>
+        <v>-1.7837871035428981E-2</v>
+      </c>
+      <c r="K32">
+        <f>IFERROR(_xlfn.RANK.EQ(J32,J$2:J$52,0),"N/A")</f>
+        <v>14</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -2708,15 +3076,19 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32" s="10">
-        <f t="shared" si="4"/>
-        <v>169827.98000000045</v>
+        <f>M32-L32</f>
+        <v>-169827.98000000045</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" si="5"/>
-        <v>2.7581118653977402E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N32)/L32,"-")</f>
+        <v>-2.7581118653977402E-2</v>
+      </c>
+      <c r="P32">
+        <f>IFERROR(_xlfn.RANK.EQ(O32,O$2:O$52,0),"N/A")</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2727,12 +3099,16 @@
         <v>920284264.73000002</v>
       </c>
       <c r="D33" s="10">
-        <f t="shared" si="0"/>
-        <v>7418835.2699990273</v>
+        <f>C33-B33</f>
+        <v>-7418835.2699990273</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" si="1"/>
-        <v>7.9969930789269058E-3</v>
+        <f>IFERROR((D33)/B33,"-")</f>
+        <v>-7.9969930789269058E-3</v>
+      </c>
+      <c r="F33">
+        <f>IFERROR(_xlfn.RANK.EQ(E33,E$2:E$52,0),"N/A")</f>
+        <v>8</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -2741,12 +3117,16 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33" s="10">
-        <f t="shared" si="2"/>
-        <v>2602486.5199999809</v>
+        <f>H33-G33</f>
+        <v>-2602486.5199999809</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6564903115433454E-3</v>
+        <f>IFERROR((I33)/G33,"-")</f>
+        <v>-2.6564903115433454E-3</v>
+      </c>
+      <c r="K33">
+        <f>IFERROR(_xlfn.RANK.EQ(J33,J$2:J$52,0),"N/A")</f>
+        <v>6</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -2755,15 +3135,19 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33" s="10">
-        <f t="shared" si="4"/>
-        <v>5456610.5900000334</v>
+        <f>M33-L33</f>
+        <v>-5456610.5900000334</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="5"/>
-        <v>5.5141067323084929E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N33)/L33,"-")</f>
+        <v>-5.5141067323084929E-3</v>
+      </c>
+      <c r="P33">
+        <f>IFERROR(_xlfn.RANK.EQ(O33,O$2:O$52,0),"N/A")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2774,12 +3158,16 @@
         <v>4109958.22</v>
       </c>
       <c r="D34" s="10">
-        <f t="shared" si="0"/>
-        <v>79341.779999999795</v>
+        <f>C34-B34</f>
+        <v>-79341.779999999795</v>
       </c>
       <c r="E34" s="5">
-        <f t="shared" si="1"/>
-        <v>1.8939149738619768E-2</v>
+        <f>IFERROR((D34)/B34,"-")</f>
+        <v>-1.8939149738619768E-2</v>
+      </c>
+      <c r="F34">
+        <f>IFERROR(_xlfn.RANK.EQ(E34,E$2:E$52,0),"N/A")</f>
+        <v>23</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -2788,12 +3176,16 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34" s="10">
-        <f t="shared" si="2"/>
-        <v>213011.23000001023</v>
+        <f>H34-G34</f>
+        <v>-213011.23000001023</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="3"/>
-        <v>4.8961345561534093E-2</v>
+        <f>IFERROR((I34)/G34,"-")</f>
+        <v>-4.8961345561534093E-2</v>
+      </c>
+      <c r="K34">
+        <f>IFERROR(_xlfn.RANK.EQ(J34,J$2:J$52,0),"N/A")</f>
+        <v>28</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -2802,15 +3194,19 @@
         <v>4229801.51</v>
       </c>
       <c r="N34" s="10">
-        <f t="shared" si="4"/>
-        <v>115798.49000000022</v>
+        <f>M34-L34</f>
+        <v>-115798.49000000022</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" si="5"/>
-        <v>2.6647296115611244E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N34)/L34,"-")</f>
+        <v>-2.6647296115611244E-2</v>
+      </c>
+      <c r="P34">
+        <f>IFERROR(_xlfn.RANK.EQ(O34,O$2:O$52,0),"N/A")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2821,12 +3217,16 @@
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <f t="shared" si="0"/>
+        <f>C35-B35</f>
         <v>0</v>
       </c>
       <c r="E35" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>IFERROR((D35)/B35,"-")</f>
         <v>-</v>
+      </c>
+      <c r="F35" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(E35,E$2:E$52,0),"N/A")</f>
+        <v>N/A</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -2835,12 +3235,16 @@
         <v>0</v>
       </c>
       <c r="I35" s="10">
-        <f t="shared" si="2"/>
+        <f>H35-G35</f>
         <v>0</v>
       </c>
       <c r="J35" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f>IFERROR((I35)/G35,"-")</f>
         <v>-</v>
+      </c>
+      <c r="K35" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(J35,J$2:J$52,0),"N/A")</f>
+        <v>N/A</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -2849,15 +3253,19 @@
         <v>0</v>
       </c>
       <c r="N35" s="10">
-        <f t="shared" si="4"/>
+        <f>M35-L35</f>
         <v>0</v>
       </c>
       <c r="O35" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f>IFERROR((N35)/L35,"-")</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(O35,O$2:O$52,0),"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2868,12 +3276,16 @@
         <v>735423.27999999898</v>
       </c>
       <c r="D36" s="10">
-        <f t="shared" si="0"/>
-        <v>62776.72000000102</v>
+        <f>C36-B36</f>
+        <v>-62776.72000000102</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="1"/>
-        <v>7.8647857679780775E-2</v>
+        <f>IFERROR((D36)/B36,"-")</f>
+        <v>-7.8647857679780775E-2</v>
+      </c>
+      <c r="F36">
+        <f>IFERROR(_xlfn.RANK.EQ(E36,E$2:E$52,0),"N/A")</f>
+        <v>39</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -2882,12 +3294,16 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36" s="10">
-        <f t="shared" si="2"/>
-        <v>157733.05000000098</v>
+        <f>H36-G36</f>
+        <v>-157733.05000000098</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="3"/>
-        <v>0.17551246244575608</v>
+        <f>IFERROR((I36)/G36,"-")</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="K36">
+        <f>IFERROR(_xlfn.RANK.EQ(J36,J$2:J$52,0),"N/A")</f>
+        <v>48</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -2896,15 +3312,19 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36" s="10">
-        <f t="shared" si="4"/>
-        <v>101084.71000000101</v>
+        <f>M36-L36</f>
+        <v>-101084.71000000101</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="5"/>
-        <v>0.11509132414892521</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N36)/L36,"-")</f>
+        <v>-0.11509132414892521</v>
+      </c>
+      <c r="P36">
+        <f>IFERROR(_xlfn.RANK.EQ(O36,O$2:O$52,0),"N/A")</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2915,12 +3335,16 @@
         <v>2005447.73999999</v>
       </c>
       <c r="D37" s="10">
-        <f t="shared" si="0"/>
-        <v>82352.260000010021</v>
+        <f>C37-B37</f>
+        <v>-82352.260000010021</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="1"/>
-        <v>3.9444515758219188E-2</v>
+        <f>IFERROR((D37)/B37,"-")</f>
+        <v>-3.9444515758219188E-2</v>
+      </c>
+      <c r="F37">
+        <f>IFERROR(_xlfn.RANK.EQ(E37,E$2:E$52,0),"N/A")</f>
+        <v>30</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -2929,12 +3353,16 @@
         <v>2118943.21</v>
       </c>
       <c r="I37" s="10">
-        <f t="shared" si="2"/>
-        <v>110256.79000000004</v>
+        <f>H37-G37</f>
+        <v>-110256.79000000004</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="3"/>
-        <v>4.9460250314014013E-2</v>
+        <f>IFERROR((I37)/G37,"-")</f>
+        <v>-4.9460250314014013E-2</v>
+      </c>
+      <c r="K37">
+        <f>IFERROR(_xlfn.RANK.EQ(J37,J$2:J$52,0),"N/A")</f>
+        <v>29</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -2943,15 +3371,19 @@
         <v>2108718.34</v>
       </c>
       <c r="N37" s="10">
-        <f t="shared" si="4"/>
-        <v>188181.66000000015</v>
+        <f>M37-L37</f>
+        <v>-188181.66000000015</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="5"/>
-        <v>8.1928538464887526E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N37)/L37,"-")</f>
+        <v>-8.1928538464887526E-2</v>
+      </c>
+      <c r="P37">
+        <f>IFERROR(_xlfn.RANK.EQ(O37,O$2:O$52,0),"N/A")</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2962,12 +3394,16 @@
         <v>838669.82</v>
       </c>
       <c r="D38" s="10">
-        <f t="shared" si="0"/>
-        <v>16630.180000000051</v>
+        <f>C38-B38</f>
+        <v>-16630.180000000051</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="1"/>
-        <v>1.9443680579913542E-2</v>
+        <f>IFERROR((D38)/B38,"-")</f>
+        <v>-1.9443680579913542E-2</v>
+      </c>
+      <c r="F38">
+        <f>IFERROR(_xlfn.RANK.EQ(E38,E$2:E$52,0),"N/A")</f>
+        <v>24</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -2976,12 +3412,16 @@
         <v>753451.96</v>
       </c>
       <c r="I38" s="10">
-        <f t="shared" si="2"/>
-        <v>39348.040000000037</v>
+        <f>H38-G38</f>
+        <v>-39348.040000000037</v>
       </c>
       <c r="J38" s="5">
-        <f t="shared" si="3"/>
-        <v>4.9631735620585316E-2</v>
+        <f>IFERROR((I38)/G38,"-")</f>
+        <v>-4.9631735620585316E-2</v>
+      </c>
+      <c r="K38">
+        <f>IFERROR(_xlfn.RANK.EQ(J38,J$2:J$52,0),"N/A")</f>
+        <v>30</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -2990,15 +3430,19 @@
         <v>777663.26</v>
       </c>
       <c r="N38" s="10">
-        <f t="shared" si="4"/>
-        <v>136.73999999999069</v>
+        <f>M38-L38</f>
+        <v>-136.73999999999069</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="5"/>
-        <v>1.7580354847003174E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N38)/L38,"-")</f>
+        <v>-1.7580354847003174E-4</v>
+      </c>
+      <c r="P38">
+        <f>IFERROR(_xlfn.RANK.EQ(O38,O$2:O$52,0),"N/A")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -3009,12 +3453,16 @@
         <v>813108.87</v>
       </c>
       <c r="D39" s="10">
-        <f t="shared" si="0"/>
-        <v>70791.13</v>
+        <f>C39-B39</f>
+        <v>-70791.13</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="1"/>
-        <v>8.008952370177623E-2</v>
+        <f>IFERROR((D39)/B39,"-")</f>
+        <v>-8.008952370177623E-2</v>
+      </c>
+      <c r="F39">
+        <f>IFERROR(_xlfn.RANK.EQ(E39,E$2:E$52,0),"N/A")</f>
+        <v>41</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3023,12 +3471,16 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39" s="10">
-        <f t="shared" si="2"/>
-        <v>180157.72000000998</v>
+        <f>H39-G39</f>
+        <v>-180157.72000000998</v>
       </c>
       <c r="J39" s="5">
-        <f t="shared" si="3"/>
-        <v>0.13918241656366656</v>
+        <f>IFERROR((I39)/G39,"-")</f>
+        <v>-0.13918241656366656</v>
+      </c>
+      <c r="K39">
+        <f>IFERROR(_xlfn.RANK.EQ(J39,J$2:J$52,0),"N/A")</f>
+        <v>46</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -3037,15 +3489,19 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39" s="10">
-        <f t="shared" si="4"/>
-        <v>79036.1300000099</v>
+        <f>M39-L39</f>
+        <v>-79036.1300000099</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="5"/>
-        <v>4.4919653310605226E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N39)/L39,"-")</f>
+        <v>-4.4919653310605226E-2</v>
+      </c>
+      <c r="P39">
+        <f>IFERROR(_xlfn.RANK.EQ(O39,O$2:O$52,0),"N/A")</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3056,12 +3512,16 @@
         <v>37565141.859999903</v>
       </c>
       <c r="D40" s="10">
-        <f t="shared" si="0"/>
-        <v>816758.14000009745</v>
+        <f>C40-B40</f>
+        <v>-816758.14000009745</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="1"/>
-        <v>2.1279773539092578E-2</v>
+        <f>IFERROR((D40)/B40,"-")</f>
+        <v>-2.1279773539092578E-2</v>
+      </c>
+      <c r="F40">
+        <f>IFERROR(_xlfn.RANK.EQ(E40,E$2:E$52,0),"N/A")</f>
+        <v>26</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3070,12 +3530,16 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40" s="10">
-        <f t="shared" si="2"/>
-        <v>1869659.8100000992</v>
+        <f>H40-G40</f>
+        <v>-1869659.8100000992</v>
       </c>
       <c r="J40" s="5">
-        <f t="shared" si="3"/>
-        <v>4.6782546934937892E-2</v>
+        <f>IFERROR((I40)/G40,"-")</f>
+        <v>-4.6782546934937892E-2</v>
+      </c>
+      <c r="K40">
+        <f>IFERROR(_xlfn.RANK.EQ(J40,J$2:J$52,0),"N/A")</f>
+        <v>27</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -3084,15 +3548,19 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40" s="10">
-        <f t="shared" si="4"/>
-        <v>610436.29000010341</v>
+        <f>M40-L40</f>
+        <v>-610436.29000010341</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="5"/>
-        <v>1.5178676768608648E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N40)/L40,"-")</f>
+        <v>-1.5178676768608648E-2</v>
+      </c>
+      <c r="P40">
+        <f>IFERROR(_xlfn.RANK.EQ(O40,O$2:O$52,0),"N/A")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3103,12 +3571,16 @@
         <v>4409060.2099999897</v>
       </c>
       <c r="D41" s="10">
-        <f t="shared" si="0"/>
-        <v>184239.79000001028</v>
+        <f>C41-B41</f>
+        <v>-184239.79000001028</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="1"/>
-        <v>4.0110550149132493E-2</v>
+        <f>IFERROR((D41)/B41,"-")</f>
+        <v>-4.0110550149132493E-2</v>
+      </c>
+      <c r="F41">
+        <f>IFERROR(_xlfn.RANK.EQ(E41,E$2:E$52,0),"N/A")</f>
+        <v>32</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3117,12 +3589,16 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41" s="10">
-        <f t="shared" si="2"/>
-        <v>133456.33000001032</v>
+        <f>H41-G41</f>
+        <v>-133456.33000001032</v>
       </c>
       <c r="J41" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6221894095689226E-2</v>
+        <f>IFERROR((I41)/G41,"-")</f>
+        <v>-2.6221894095689226E-2</v>
+      </c>
+      <c r="K41">
+        <f>IFERROR(_xlfn.RANK.EQ(J41,J$2:J$52,0),"N/A")</f>
+        <v>15</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -3131,15 +3607,19 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41" s="10">
-        <f t="shared" si="4"/>
-        <v>82077.349999999627</v>
+        <f>M41-L41</f>
+        <v>-82077.349999999627</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="5"/>
-        <v>1.7099804162586642E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N41)/L41,"-")</f>
+        <v>-1.7099804162586642E-2</v>
+      </c>
+      <c r="P41">
+        <f>IFERROR(_xlfn.RANK.EQ(O41,O$2:O$52,0),"N/A")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -3150,12 +3630,16 @@
         <v>188551675.67999899</v>
       </c>
       <c r="D42" s="10">
-        <f t="shared" si="0"/>
-        <v>41624.320001006126</v>
+        <f>C42-B42</f>
+        <v>-41624.320001006126</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="1"/>
-        <v>2.2070943135841053E-4</v>
+        <f>IFERROR((D42)/B42,"-")</f>
+        <v>-2.2070943135841053E-4</v>
+      </c>
+      <c r="F42">
+        <f>IFERROR(_xlfn.RANK.EQ(E42,E$2:E$52,0),"N/A")</f>
+        <v>5</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3164,12 +3648,16 @@
         <v>196755033.31</v>
       </c>
       <c r="I42" s="10">
-        <f t="shared" si="2"/>
-        <v>2375266.6899999976</v>
+        <f>H42-G42</f>
+        <v>-2375266.6899999976</v>
       </c>
       <c r="J42" s="5">
-        <f t="shared" si="3"/>
-        <v>1.1928203241796942E-2</v>
+        <f>IFERROR((I42)/G42,"-")</f>
+        <v>-1.1928203241796942E-2</v>
+      </c>
+      <c r="K42">
+        <f>IFERROR(_xlfn.RANK.EQ(J42,J$2:J$52,0),"N/A")</f>
+        <v>10</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -3178,15 +3666,19 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42" s="10">
-        <f t="shared" si="4"/>
-        <v>36.250001013278961</v>
+        <f>M42-L42</f>
+        <v>-36.250001013278961</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="5"/>
-        <v>1.8129115815929696E-7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N42)/L42,"-")</f>
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="P42">
+        <f>IFERROR(_xlfn.RANK.EQ(O42,O$2:O$52,0),"N/A")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -3197,12 +3689,16 @@
         <v>7968645.8300000001</v>
       </c>
       <c r="D43" s="10">
-        <f t="shared" si="0"/>
-        <v>166754.16999999993</v>
+        <f>C43-B43</f>
+        <v>-166754.16999999993</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="1"/>
-        <v>2.0497353541313264E-2</v>
+        <f>IFERROR((D43)/B43,"-")</f>
+        <v>-2.0497353541313264E-2</v>
+      </c>
+      <c r="F43">
+        <f>IFERROR(_xlfn.RANK.EQ(E43,E$2:E$52,0),"N/A")</f>
+        <v>25</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3211,12 +3707,16 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43" s="10">
-        <f t="shared" si="2"/>
-        <v>389327.98000000045</v>
+        <f>H43-G43</f>
+        <v>-389327.98000000045</v>
       </c>
       <c r="J43" s="5">
-        <f t="shared" si="3"/>
-        <v>4.5477990374731388E-2</v>
+        <f>IFERROR((I43)/G43,"-")</f>
+        <v>-4.5477990374731388E-2</v>
+      </c>
+      <c r="K43">
+        <f>IFERROR(_xlfn.RANK.EQ(J43,J$2:J$52,0),"N/A")</f>
+        <v>26</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -3225,15 +3725,19 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43" s="10">
-        <f t="shared" si="4"/>
-        <v>346517.43000000995</v>
+        <f>M43-L43</f>
+        <v>-346517.43000000995</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="5"/>
-        <v>4.0778750220654303E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N43)/L43,"-")</f>
+        <v>-4.0778750220654303E-2</v>
+      </c>
+      <c r="P43">
+        <f>IFERROR(_xlfn.RANK.EQ(O43,O$2:O$52,0),"N/A")</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -3244,12 +3748,16 @@
         <v>29789104.379999999</v>
       </c>
       <c r="D44" s="10">
-        <f t="shared" si="0"/>
-        <v>294095.62000000104</v>
+        <f>C44-B44</f>
+        <v>-294095.62000000104</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="1"/>
-        <v>9.7760750186150751E-3</v>
+        <f>IFERROR((D44)/B44,"-")</f>
+        <v>-9.7760750186150751E-3</v>
+      </c>
+      <c r="F44">
+        <f>IFERROR(_xlfn.RANK.EQ(E44,E$2:E$52,0),"N/A")</f>
+        <v>10</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3258,12 +3766,16 @@
         <v>30793711.48</v>
       </c>
       <c r="I44" s="10">
-        <f t="shared" si="2"/>
-        <v>246988.51999999955</v>
+        <f>H44-G44</f>
+        <v>-246988.51999999955</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="3"/>
-        <v>7.9569249404813532E-3</v>
+        <f>IFERROR((I44)/G44,"-")</f>
+        <v>-7.9569249404813532E-3</v>
+      </c>
+      <c r="K44">
+        <f>IFERROR(_xlfn.RANK.EQ(J44,J$2:J$52,0),"N/A")</f>
+        <v>8</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -3272,15 +3784,19 @@
         <v>31282141.25</v>
       </c>
       <c r="N44" s="10">
-        <f t="shared" si="4"/>
-        <v>58.75</v>
+        <f>M44-L44</f>
+        <v>-58.75</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="5"/>
-        <v>1.8780648419868168E-6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N44)/L44,"-")</f>
+        <v>-1.8780648419868168E-6</v>
+      </c>
+      <c r="P44">
+        <f>IFERROR(_xlfn.RANK.EQ(O44,O$2:O$52,0),"N/A")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -3291,12 +3807,16 @@
         <v>54589584.0499999</v>
       </c>
       <c r="D45" s="10">
-        <f t="shared" si="0"/>
-        <v>712015.95000009984</v>
+        <f>C45-B45</f>
+        <v>-712015.95000009984</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="1"/>
-        <v>1.287514194887851E-2</v>
+        <f>IFERROR((D45)/B45,"-")</f>
+        <v>-1.287514194887851E-2</v>
+      </c>
+      <c r="F45">
+        <f>IFERROR(_xlfn.RANK.EQ(E45,E$2:E$52,0),"N/A")</f>
+        <v>15</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3305,12 +3825,16 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45" s="10">
-        <f t="shared" si="2"/>
-        <v>2197246.0400001034</v>
+        <f>H45-G45</f>
+        <v>-2197246.0400001034</v>
       </c>
       <c r="J45" s="5">
-        <f t="shared" si="3"/>
-        <v>3.8689222111488959E-2</v>
+        <f>IFERROR((I45)/G45,"-")</f>
+        <v>-3.8689222111488959E-2</v>
+      </c>
+      <c r="K45">
+        <f>IFERROR(_xlfn.RANK.EQ(J45,J$2:J$52,0),"N/A")</f>
+        <v>19</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -3319,15 +3843,19 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45" s="10">
-        <f t="shared" si="4"/>
-        <v>640550.34000010043</v>
+        <f>M45-L45</f>
+        <v>-640550.34000010043</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="5"/>
-        <v>1.1432866237947358E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N45)/L45,"-")</f>
+        <v>-1.1432866237947358E-2</v>
+      </c>
+      <c r="P45">
+        <f>IFERROR(_xlfn.RANK.EQ(O45,O$2:O$52,0),"N/A")</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -3338,12 +3866,16 @@
         <v>258322.43</v>
       </c>
       <c r="D46" s="10">
-        <f t="shared" si="0"/>
-        <v>777.57000000000698</v>
+        <f>C46-B46</f>
+        <v>-777.57000000000698</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="1"/>
-        <v>3.0010420686993711E-3</v>
+        <f>IFERROR((D46)/B46,"-")</f>
+        <v>-3.0010420686993711E-3</v>
+      </c>
+      <c r="F46">
+        <f>IFERROR(_xlfn.RANK.EQ(E46,E$2:E$52,0),"N/A")</f>
+        <v>6</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3352,12 +3884,16 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46" s="10">
-        <f t="shared" si="2"/>
-        <v>8597.090000000986</v>
+        <f>H46-G46</f>
+        <v>-8597.090000000986</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="3"/>
-        <v>3.2319887218048821E-2</v>
+        <f>IFERROR((I46)/G46,"-")</f>
+        <v>-3.2319887218048821E-2</v>
+      </c>
+      <c r="K46">
+        <f>IFERROR(_xlfn.RANK.EQ(J46,J$2:J$52,0),"N/A")</f>
+        <v>16</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -3366,15 +3902,19 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46" s="10">
-        <f t="shared" si="4"/>
-        <v>12346.840000000986</v>
+        <f>M46-L46</f>
+        <v>-12346.840000000986</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="5"/>
-        <v>4.6225533508053113E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N46)/L46,"-")</f>
+        <v>-4.6225533508053113E-2</v>
+      </c>
+      <c r="P46">
+        <f>IFERROR(_xlfn.RANK.EQ(O46,O$2:O$52,0),"N/A")</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -3385,12 +3925,16 @@
         <v>70378426.719999999</v>
       </c>
       <c r="D47" s="10">
-        <f t="shared" si="0"/>
-        <v>12273.280000001192</v>
+        <f>C47-B47</f>
+        <v>-12273.280000001192</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="1"/>
-        <v>1.7435939690898361E-4</v>
+        <f>IFERROR((D47)/B47,"-")</f>
+        <v>-1.7435939690898361E-4</v>
+      </c>
+      <c r="F47">
+        <f>IFERROR(_xlfn.RANK.EQ(E47,E$2:E$52,0),"N/A")</f>
+        <v>4</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3399,12 +3943,16 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47" s="10">
-        <f t="shared" si="2"/>
-        <v>24458.340000003576</v>
+        <f>H47-G47</f>
+        <v>-24458.340000003576</v>
       </c>
       <c r="J47" s="5">
-        <f t="shared" si="3"/>
-        <v>3.3291600310348285E-4</v>
+        <f>IFERROR((I47)/G47,"-")</f>
+        <v>-3.3291600310348285E-4</v>
+      </c>
+      <c r="K47">
+        <f>IFERROR(_xlfn.RANK.EQ(J47,J$2:J$52,0),"N/A")</f>
+        <v>4</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -3413,15 +3961,19 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47" s="10">
-        <f t="shared" si="4"/>
-        <v>21970.820000097156</v>
+        <f>M47-L47</f>
+        <v>-21970.820000097156</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="5"/>
-        <v>2.9266019117572752E-4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N47)/L47,"-")</f>
+        <v>-2.9266019117572752E-4</v>
+      </c>
+      <c r="P47">
+        <f>IFERROR(_xlfn.RANK.EQ(O47,O$2:O$52,0),"N/A")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -3432,12 +3984,16 @@
         <v>6527352.5699999901</v>
       </c>
       <c r="D48" s="10">
-        <f t="shared" si="0"/>
-        <v>209747.43000000995</v>
+        <f>C48-B48</f>
+        <v>-209747.43000000995</v>
       </c>
       <c r="E48" s="5">
-        <f t="shared" si="1"/>
-        <v>3.1133192323107857E-2</v>
+        <f>IFERROR((D48)/B48,"-")</f>
+        <v>-3.1133192323107857E-2</v>
+      </c>
+      <c r="F48">
+        <f>IFERROR(_xlfn.RANK.EQ(E48,E$2:E$52,0),"N/A")</f>
+        <v>29</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -3446,12 +4002,16 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48" s="10">
-        <f t="shared" si="2"/>
-        <v>292627.44000000041</v>
+        <f>H48-G48</f>
+        <v>-292627.44000000041</v>
       </c>
       <c r="J48" s="5">
-        <f t="shared" si="3"/>
-        <v>4.0559890224125802E-2</v>
+        <f>IFERROR((I48)/G48,"-")</f>
+        <v>-4.0559890224125802E-2</v>
+      </c>
+      <c r="K48">
+        <f>IFERROR(_xlfn.RANK.EQ(J48,J$2:J$52,0),"N/A")</f>
+        <v>20</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -3460,15 +4020,19 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48" s="10">
-        <f t="shared" si="4"/>
-        <v>407449.76000001002</v>
+        <f>M48-L48</f>
+        <v>-407449.76000001002</v>
       </c>
       <c r="O48" s="5">
-        <f t="shared" si="5"/>
-        <v>5.5893132870587676E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N48)/L48,"-")</f>
+        <v>-5.5893132870587676E-2</v>
+      </c>
+      <c r="P48">
+        <f>IFERROR(_xlfn.RANK.EQ(O48,O$2:O$52,0),"N/A")</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -3479,12 +4043,16 @@
         <v>90499.43</v>
       </c>
       <c r="D49" s="10">
-        <f t="shared" si="0"/>
-        <v>1700.570000000007</v>
+        <f>C49-B49</f>
+        <v>-1700.570000000007</v>
       </c>
       <c r="E49" s="5">
-        <f t="shared" si="1"/>
-        <v>1.8444360086767971E-2</v>
+        <f>IFERROR((D49)/B49,"-")</f>
+        <v>-1.8444360086767971E-2</v>
+      </c>
+      <c r="F49">
+        <f>IFERROR(_xlfn.RANK.EQ(E49,E$2:E$52,0),"N/A")</f>
+        <v>22</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -3493,12 +4061,16 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49" s="10">
-        <f t="shared" si="2"/>
-        <v>7133.1199999999953</v>
+        <f>H49-G49</f>
+        <v>-7133.1199999999953</v>
       </c>
       <c r="J49" s="5">
-        <f t="shared" si="3"/>
-        <v>6.9523586744639335E-2</v>
+        <f>IFERROR((I49)/G49,"-")</f>
+        <v>-6.9523586744639335E-2</v>
+      </c>
+      <c r="K49">
+        <f>IFERROR(_xlfn.RANK.EQ(J49,J$2:J$52,0),"N/A")</f>
+        <v>36</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -3507,15 +4079,19 @@
         <v>0</v>
       </c>
       <c r="N49" s="10">
-        <f t="shared" si="4"/>
+        <f>M49-L49</f>
         <v>0</v>
       </c>
       <c r="O49" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f>IFERROR((N49)/L49,"-")</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49" t="str">
+        <f>IFERROR(_xlfn.RANK.EQ(O49,O$2:O$52,0),"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -3526,12 +4102,16 @@
         <v>832600</v>
       </c>
       <c r="D50" s="10">
-        <f t="shared" si="0"/>
+        <f>C50-B50</f>
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <f t="shared" si="1"/>
+        <f>IFERROR((D50)/B50,"-")</f>
         <v>0</v>
+      </c>
+      <c r="F50">
+        <f>IFERROR(_xlfn.RANK.EQ(E50,E$2:E$52,0),"N/A")</f>
+        <v>2</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -3540,12 +4120,16 @@
         <v>859100</v>
       </c>
       <c r="I50" s="10">
-        <f t="shared" si="2"/>
+        <f>H50-G50</f>
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" si="3"/>
+        <f>IFERROR((I50)/G50,"-")</f>
         <v>0</v>
+      </c>
+      <c r="K50">
+        <f>IFERROR(_xlfn.RANK.EQ(J50,J$2:J$52,0),"N/A")</f>
+        <v>1</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -3554,15 +4138,19 @@
         <v>843200</v>
       </c>
       <c r="N50" s="10">
-        <f t="shared" si="4"/>
+        <f>M50-L50</f>
         <v>0</v>
       </c>
       <c r="O50" s="5">
-        <f t="shared" si="5"/>
+        <f>IFERROR((N50)/L50,"-")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50">
+        <f>IFERROR(_xlfn.RANK.EQ(O50,O$2:O$52,0),"N/A")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -3573,12 +4161,16 @@
         <v>8499425.3399999905</v>
       </c>
       <c r="D51" s="10">
-        <f t="shared" si="0"/>
-        <v>110074.66000000946</v>
+        <f>C51-B51</f>
+        <v>-110074.66000000946</v>
       </c>
       <c r="E51" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2785255822058129E-2</v>
+        <f>IFERROR((D51)/B51,"-")</f>
+        <v>-1.2785255822058129E-2</v>
+      </c>
+      <c r="F51">
+        <f>IFERROR(_xlfn.RANK.EQ(E51,E$2:E$52,0),"N/A")</f>
+        <v>14</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -3587,12 +4179,16 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51" s="10">
-        <f t="shared" si="2"/>
-        <v>326440.38000000082</v>
+        <f>H51-G51</f>
+        <v>-326440.38000000082</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="3"/>
-        <v>3.6573903982970231E-2</v>
+        <f>IFERROR((I51)/G51,"-")</f>
+        <v>-3.6573903982970231E-2</v>
+      </c>
+      <c r="K51">
+        <f>IFERROR(_xlfn.RANK.EQ(J51,J$2:J$52,0),"N/A")</f>
+        <v>18</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -3601,15 +4197,19 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51" s="10">
-        <f t="shared" si="4"/>
-        <v>98056.689999999478</v>
+        <f>M51-L51</f>
+        <v>-98056.689999999478</v>
       </c>
       <c r="O51" s="5">
-        <f t="shared" si="5"/>
-        <v>1.1100045280114048E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N51)/L51,"-")</f>
+        <v>-1.1100045280114048E-2</v>
+      </c>
+      <c r="P51">
+        <f>IFERROR(_xlfn.RANK.EQ(O51,O$2:O$52,0),"N/A")</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -3620,12 +4220,16 @@
         <v>2254684.7999999998</v>
       </c>
       <c r="D52" s="10">
-        <f t="shared" si="0"/>
-        <v>196315.20000000019</v>
+        <f>C52-B52</f>
+        <v>-196315.20000000019</v>
       </c>
       <c r="E52" s="5">
-        <f t="shared" si="1"/>
-        <v>8.009596083231342E-2</v>
+        <f>IFERROR((D52)/B52,"-")</f>
+        <v>-8.009596083231342E-2</v>
+      </c>
+      <c r="F52">
+        <f>IFERROR(_xlfn.RANK.EQ(E52,E$2:E$52,0),"N/A")</f>
+        <v>42</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -3634,12 +4238,16 @@
         <v>2204672.88</v>
       </c>
       <c r="I52" s="10">
-        <f t="shared" si="2"/>
-        <v>236027.12000000011</v>
+        <f>H52-G52</f>
+        <v>-236027.12000000011</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="3"/>
-        <v>9.6704683082722218E-2</v>
+        <f>IFERROR((I52)/G52,"-")</f>
+        <v>-9.6704683082722218E-2</v>
+      </c>
+      <c r="K52">
+        <f>IFERROR(_xlfn.RANK.EQ(J52,J$2:J$52,0),"N/A")</f>
+        <v>40</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -3648,20 +4256,24 @@
         <v>2056835.26</v>
       </c>
       <c r="N52" s="10">
-        <f t="shared" si="4"/>
-        <v>264764.74</v>
+        <f>M52-L52</f>
+        <v>-264764.74</v>
       </c>
       <c r="O52" s="5">
-        <f t="shared" si="5"/>
-        <v>0.11404408166781529</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IFERROR((N52)/L52,"-")</f>
+        <v>-0.11404408166781529</v>
+      </c>
+      <c r="P52">
+        <f>IFERROR(_xlfn.RANK.EQ(O52,O$2:O$52,0),"N/A")</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -3675,42 +4287,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>